<commit_message>
CHP study reports updated
</commit_message>
<xml_diff>
--- a/Reports/CHP-study/chp-org.xlsx
+++ b/Reports/CHP-study/chp-org.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHP\Reports\CHP-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4294834D-6082-4181-A9AB-1928C7D94904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6F7B67-577F-4B26-BE49-E710294530AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rev 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t>Shri D M Jha</t>
   </si>
@@ -140,12 +140,15 @@
     <t>Firefighting,
 Pumps &amp; Pipelines</t>
   </si>
+  <si>
+    <t>DUDHICHUA CHP  ORGANISATION CHART</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +199,37 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -408,6 +442,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -420,93 +481,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -519,29 +550,131 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3625,13 +3758,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -3731,7 +3864,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -3743,7 +3876,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="18"/>
       <c r="F28" s="2" t="s">
         <v>14</v>
       </c>
@@ -3753,7 +3886,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="10"/>
+      <c r="D29" s="19"/>
       <c r="F29" s="3" t="s">
         <v>15</v>
       </c>
@@ -3801,88 +3934,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="12" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="13" style="12" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="15" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="4.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="13" style="8" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="39"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
@@ -3900,52 +4033,52 @@
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="30"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="39"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
@@ -3963,54 +4096,54 @@
     </row>
     <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
@@ -4028,180 +4161,185 @@
     </row>
     <row r="17" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="37"/>
     </row>
     <row r="19" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="45" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="47"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="F26" s="27" t="s">
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="F26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="I26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="26" t="s">
+      <c r="L26" s="10"/>
+      <c r="M26" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="26"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
     </row>
     <row r="30" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
     </row>
     <row r="31" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B19:K19"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="I26:I28"/>
     <mergeCell ref="J26:J28"/>
@@ -4218,11 +4356,6 @@
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:M10"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B18:K18"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B19:K19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4238,476 +4371,657 @@
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="12" customWidth="1"/>
-    <col min="9" max="10" width="12.28515625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="15" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="4.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="8" customWidth="1"/>
+    <col min="9" max="10" width="12.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-    </row>
-    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+    <row r="1" spans="1:17" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+    </row>
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="45"/>
+    </row>
+    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="45"/>
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="30"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="45"/>
     </row>
     <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="39"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="45"/>
     </row>
     <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="33"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="55"/>
+      <c r="P5" s="45"/>
     </row>
     <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="45"/>
+    </row>
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="45"/>
+    </row>
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="45"/>
+      <c r="B8" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="30"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="45"/>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="39"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="45"/>
     </row>
     <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="33"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="45"/>
     </row>
     <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="45"/>
+    </row>
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="45"/>
+    </row>
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="45"/>
+      <c r="B13" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="36"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="33"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="45"/>
+    </row>
+    <row r="17" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="45"/>
+    </row>
+    <row r="18" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="45"/>
+      <c r="B18" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-    </row>
-    <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="14"/>
-    </row>
-    <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="45"/>
+    </row>
+    <row r="21" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="45"/>
+    </row>
+    <row r="22" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="45"/>
+      <c r="B22" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="72"/>
+      <c r="D22" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="L22" s="28" t="s">
+      <c r="E22" s="46"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="M22" s="30"/>
-    </row>
-    <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="M22" s="49"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="45"/>
+    </row>
+    <row r="23" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="45" t="s">
+      <c r="C23" s="72"/>
+      <c r="D23" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="L23" s="46" t="s">
+      <c r="E23" s="46"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="47"/>
-    </row>
-    <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="M23" s="75"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="45"/>
+    </row>
+    <row r="24" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="45"/>
+    </row>
+    <row r="25" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="45"/>
+    </row>
+    <row r="26" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45"/>
+      <c r="B26" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="F26" s="26" t="s">
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="52"/>
-      <c r="I26" s="21" t="s">
+      <c r="H26" s="78"/>
+      <c r="I26" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="27" t="s">
+      <c r="J26" s="80"/>
+      <c r="K26" s="81"/>
+      <c r="L26" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="27" t="s">
+      <c r="M26" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="N26" s="14"/>
-      <c r="O26" s="26" t="s">
+      <c r="N26" s="69"/>
+      <c r="O26" s="77" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="26"/>
-    </row>
-    <row r="28" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="26"/>
-    </row>
-    <row r="29" spans="2:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-    </row>
-    <row r="30" spans="2:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-    </row>
-    <row r="31" spans="2:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="P26" s="45"/>
+    </row>
+    <row r="27" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="45"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="45"/>
+    </row>
+    <row r="28" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="77"/>
+      <c r="P28" s="45"/>
+    </row>
+    <row r="29" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B4:O4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="B8:O8"/>
+    <mergeCell ref="B9:O9"/>
+    <mergeCell ref="B10:O10"/>
+    <mergeCell ref="B13:O13"/>
+    <mergeCell ref="B14:O14"/>
+    <mergeCell ref="B15:O15"/>
+    <mergeCell ref="B18:I18"/>
     <mergeCell ref="O26:O28"/>
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="L23:M23"/>
@@ -4717,18 +5031,6 @@
     <mergeCell ref="G26:G28"/>
     <mergeCell ref="L26:L28"/>
     <mergeCell ref="M26:M28"/>
-    <mergeCell ref="B10:O10"/>
-    <mergeCell ref="B13:O13"/>
-    <mergeCell ref="B14:O14"/>
-    <mergeCell ref="B15:O15"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B4:O4"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="B8:O8"/>
-    <mergeCell ref="B9:O9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4744,421 +5046,578 @@
   </sheetPr>
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="14" style="12" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="13" style="12" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="15" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="4.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="14" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="20" style="8" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="13" style="8" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-    </row>
-    <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="45"/>
+    </row>
+    <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="45"/>
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="39"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="45"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="45"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="45"/>
+    </row>
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="45"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="45"/>
+      <c r="B8" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="30"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="45"/>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="39"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="45"/>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="45"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="45"/>
+    </row>
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="45"/>
+    </row>
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="45"/>
+      <c r="B13" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="45"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="33"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="45"/>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="45"/>
+    </row>
+    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="45"/>
+    </row>
+    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="45"/>
+      <c r="B18" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-    </row>
-    <row r="19" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="45"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
-    </row>
-    <row r="20" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="45"/>
+    </row>
+    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="45"/>
+    </row>
+    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="45"/>
+    </row>
+    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="45"/>
+      <c r="B22" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="72"/>
+      <c r="D22" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="E22" s="46"/>
+      <c r="F22" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="G22" s="49"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="45"/>
+    </row>
+    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="45" t="s">
+      <c r="C23" s="72"/>
+      <c r="D23" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="E23" s="46"/>
+      <c r="F23" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="47"/>
-    </row>
-    <row r="24" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="G23" s="75"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="45"/>
+    </row>
+    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="45"/>
+    </row>
+    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="45"/>
+    </row>
+    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45"/>
+      <c r="B26" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="F26" s="27" t="s">
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="H26" s="46"/>
+      <c r="I26" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="26" t="s">
+      <c r="L26" s="69"/>
+      <c r="M26" s="77" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="26"/>
-    </row>
-    <row r="28" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="26"/>
-    </row>
-    <row r="29" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="N26" s="45"/>
+    </row>
+    <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="45"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="77"/>
+      <c r="N27" s="45"/>
+    </row>
+    <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="77"/>
+      <c r="N28" s="45"/>
+    </row>
+    <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+    </row>
+    <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="K26:K28"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B8:M8"/>
     <mergeCell ref="B26:D28"/>
     <mergeCell ref="F26:F28"/>
     <mergeCell ref="G26:G28"/>
@@ -5169,16 +5628,15 @@
     <mergeCell ref="B15:M15"/>
     <mergeCell ref="B18:M18"/>
     <mergeCell ref="B19:M19"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>